<commit_message>
backlog geupdate, unused usings verwijderd
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Case_BPM2\Case_BPM3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E65E4C01-817F-49F6-B688-1348F3B91489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A331F9-C51E-4218-8ACC-0D4802BABB9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="1284" windowWidth="17280" windowHeight="8964" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="137">
   <si>
     <t>Cursussen invoeren</t>
   </si>
@@ -576,10 +576,31 @@
     <t>Angular frontend opzetten en ttoevoegen aan de repo</t>
   </si>
   <si>
-    <t>Unit tests toevoegen voor gebouwde functionaliteit</t>
-  </si>
-  <si>
-    <t>Is erg veel</t>
+    <t>Unit tests voor cursus service uitbreiden</t>
+  </si>
+  <si>
+    <t>Unit test voor cursus parser service</t>
+  </si>
+  <si>
+    <t>Unit test voor de foutmeldingen service</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Refactoring van componenten en services om unit testbaar te worden</t>
+  </si>
+  <si>
+    <t>repository gebruiken</t>
+  </si>
+  <si>
+    <t>Repository gebruiken in de backend</t>
+  </si>
+  <si>
+    <t>repository unit tests</t>
+  </si>
+  <si>
+    <t>Unit tests voor oude controller omschrijven naar repository</t>
   </si>
 </sst>
 </file>
@@ -640,7 +661,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,25 +718,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -830,7 +833,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -902,6 +905,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -962,14 +968,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1340,11 +1339,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
       <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1388,14 +1387,14 @@
       <c r="AH2"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
     </row>
     <row r="4" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1488,11 +1487,11 @@
       <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
       <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
@@ -1516,9 +1515,9 @@
       <c r="AJ8" s="4"/>
     </row>
     <row r="9" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
       <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
@@ -1544,11 +1543,11 @@
       <c r="AJ10" s="22"/>
     </row>
     <row r="11" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
       <c r="I11" s="17" t="s">
         <v>38</v>
       </c>
@@ -1566,9 +1565,9 @@
       <c r="AJ11" s="4"/>
     </row>
     <row r="12" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
       <c r="I12" s="7" t="s">
         <v>39</v>
       </c>
@@ -1586,9 +1585,9 @@
       <c r="AJ12" s="4"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
       <c r="J13" s="4"/>
       <c r="W13"/>
       <c r="X13"/>
@@ -1597,9 +1596,9 @@
       <c r="AJ13" s="4"/>
     </row>
     <row r="14" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
       <c r="J14" s="4"/>
       <c r="S14" s="17" t="s">
         <v>27</v>
@@ -1614,11 +1613,11 @@
       <c r="AJ14" s="4"/>
     </row>
     <row r="15" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
       <c r="J15" s="4"/>
-      <c r="S15" s="43" t="s">
+      <c r="S15" s="46" t="s">
         <v>83</v>
       </c>
       <c r="U15" s="19" t="s">
@@ -1633,16 +1632,16 @@
     <row r="16" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
-      <c r="S16" s="44"/>
+      <c r="S16" s="47"/>
       <c r="AI16" s="22"/>
       <c r="AJ16" s="22"/>
     </row>
     <row r="17" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
       <c r="I17" s="17" t="s">
         <v>48</v>
       </c>
@@ -1654,9 +1653,9 @@
       <c r="AJ17" s="4"/>
     </row>
     <row r="18" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
       <c r="I18" s="8" t="s">
         <v>49</v>
       </c>
@@ -1668,9 +1667,9 @@
       <c r="AJ18" s="4"/>
     </row>
     <row r="19" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="W19"/>
@@ -1680,9 +1679,9 @@
       <c r="AJ19" s="4"/>
     </row>
     <row r="20" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
       <c r="G20" s="17" t="s">
         <v>56</v>
       </c>
@@ -1697,9 +1696,9 @@
       <c r="AJ20" s="4"/>
     </row>
     <row r="21" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
       <c r="G21" s="18"/>
       <c r="I21" s="19" t="s">
         <v>58</v>
@@ -1712,9 +1711,9 @@
       <c r="AJ21" s="4"/>
     </row>
     <row r="22" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="W22"/>
@@ -1724,9 +1723,9 @@
       <c r="AJ22" s="4"/>
     </row>
     <row r="23" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="42"/>
       <c r="G23" s="17" t="s">
         <v>80</v>
       </c>
@@ -1739,9 +1738,9 @@
       <c r="AJ23" s="4"/>
     </row>
     <row r="24" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="42"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="45"/>
       <c r="G24" s="19" t="s">
         <v>81</v>
       </c>
@@ -1779,11 +1778,11 @@
       <c r="AJ25" s="22"/>
     </row>
     <row r="26" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
       <c r="G26" s="17" t="s">
         <v>64</v>
       </c>
@@ -1802,9 +1801,9 @@
       <c r="AJ26" s="4"/>
     </row>
     <row r="27" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="42"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
       <c r="G27" s="18"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1827,11 +1826,11 @@
       <c r="AJ28" s="22"/>
     </row>
     <row r="29" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
       <c r="J29" s="4"/>
       <c r="W29" s="17" t="s">
         <v>8</v>
@@ -1848,9 +1847,9 @@
       <c r="AJ29" s="4"/>
     </row>
     <row r="30" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
       <c r="J30" s="4"/>
       <c r="W30" s="8" t="s">
         <v>30</v>
@@ -1866,9 +1865,9 @@
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="36"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
       <c r="I32" s="17" t="s">
         <v>70</v>
       </c>
@@ -1879,9 +1878,9 @@
       <c r="AH32" s="4"/>
     </row>
     <row r="33" spans="1:34" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="42"/>
       <c r="I33" s="19" t="s">
         <v>71</v>
       </c>
@@ -1892,9 +1891,9 @@
       <c r="AH33" s="4"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A34" s="37"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="42"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -1913,9 +1912,9 @@
       <c r="AH34" s="4"/>
     </row>
     <row r="35" spans="1:34" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="39"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="42"/>
       <c r="K35" s="17" t="s">
         <v>8</v>
       </c>
@@ -1932,9 +1931,9 @@
       <c r="AH35" s="4"/>
     </row>
     <row r="36" spans="1:34" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="42"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
       <c r="K36" s="8" t="s">
         <v>30</v>
       </c>
@@ -2234,10 +2233,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,7 +2246,7 @@
     <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="188.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
@@ -2282,639 +2281,570 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="48">
+    <row r="2" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="25">
         <v>1</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="48" t="s">
+    <row r="3" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="25" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="48" t="s">
+    <row r="4" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="25" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="26">
         <v>1</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="26">
         <v>1</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="50">
+    <row r="6" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="27">
         <v>1</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="27" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="49">
+    <row r="7" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="26">
         <v>1</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="26">
         <v>2</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="26">
         <v>2</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="49" t="s">
+      <c r="H8" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="26">
         <v>2</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="26">
         <v>2</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47">
-        <v>8</v>
-      </c>
-      <c r="C10" s="47">
+    <row r="10" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="26">
         <v>2</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D11" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E11" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F11" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="47" t="s">
+    </row>
+    <row r="12" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="26">
+        <v>2</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="26" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+    <row r="13" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="26">
+        <v>2</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B14" s="48">
         <v>2</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C14" s="48">
         <v>2</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D14" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E14" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F14" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G14" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="51" t="s">
+      <c r="H14" s="48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52" t="s">
+    <row r="15" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B15" s="26">
         <v>3</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C15" s="26">
         <v>1</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D15" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F15" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="52" t="s">
+      <c r="G15" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="52" t="s">
+      <c r="H15" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
+    <row r="16" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B16" s="26">
         <v>4</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C16" s="26">
         <v>2</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D16" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E16" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="52" t="s">
+      <c r="F16" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="52" t="s">
+      <c r="G16" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="52" t="s">
+      <c r="H16" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+    <row r="17" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B17" s="26">
         <v>4</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C17" s="26">
         <v>2</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D17" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F17" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="46" t="s">
+      <c r="G17" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="46" t="s">
+      <c r="H17" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="45" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+    <row r="18" spans="1:8" s="26" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B18" s="26">
         <v>5</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C18" s="26">
         <v>2</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D18" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E18" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="F18" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G18" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H18" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+    <row r="19" spans="1:8" s="26" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="26" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B21" s="48">
         <v>5</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C21" s="48">
         <v>2</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D21" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E21" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F21" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G21" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H21" s="48" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="23">
-        <v>8</v>
-      </c>
-      <c r="C20" s="23">
-        <v>1</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="H22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23" s="23">
-        <v>10</v>
-      </c>
-      <c r="C23" s="23">
-        <v>2</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="H24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B25">
-        <v>11</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" t="s">
+    <row r="25" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="23">
+        <v>8</v>
+      </c>
+      <c r="C25" s="23">
+        <v>1</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" s="23">
-        <v>11</v>
-      </c>
-      <c r="C26" s="23">
-        <v>3</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="23" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="H27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28">
-        <v>12</v>
-      </c>
-      <c r="C28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="23">
+        <v>10</v>
+      </c>
+      <c r="C28" s="23">
+        <v>2</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" t="s">
-        <v>23</v>
+      <c r="F28" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B29">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H29" t="s">
         <v>23</v>
@@ -2922,129 +2852,123 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B30">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31">
-        <v>14</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H31" t="s">
+    <row r="31" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="23">
+        <v>11</v>
+      </c>
+      <c r="C31" s="23">
+        <v>3</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
         <v>4</v>
       </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="H32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="23">
-        <v>14</v>
-      </c>
-      <c r="C33" s="23">
-        <v>4</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="23" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33">
         <v>12</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" s="23" t="s">
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B34">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G34" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H34" t="s">
         <v>23</v>
@@ -3052,25 +2976,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B35">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E35" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="H35" t="s">
         <v>23</v>
@@ -3078,79 +3002,79 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="H36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="H37" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38">
-        <v>16</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" t="s">
-        <v>40</v>
-      </c>
-      <c r="H38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="23">
+        <v>14</v>
+      </c>
+      <c r="C38" s="23">
+        <v>4</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H38" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3159,22 +3083,22 @@
         <v>109</v>
       </c>
       <c r="B39">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H39" t="s">
         <v>23</v>
@@ -3182,10 +3106,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B40">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -3194,13 +3118,13 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H40" t="s">
         <v>23</v>
@@ -3208,79 +3132,209 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B41">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
         <v>3</v>
       </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>21</v>
-      </c>
       <c r="F41" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="G41" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="H41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B42">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F42" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="G42" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="H42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" t="s">
+        <v>40</v>
+      </c>
+      <c r="H43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44">
+        <v>16</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G44" t="s">
+        <v>51</v>
+      </c>
+      <c r="H44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" t="s">
+        <v>59</v>
+      </c>
+      <c r="H45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>111</v>
       </c>
-      <c r="B43">
+      <c r="B47">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
         <v>19</v>
       </c>
-      <c r="C43">
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" t="s">
+        <v>59</v>
+      </c>
+      <c r="H47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48">
+        <v>19</v>
+      </c>
+      <c r="C48">
         <v>3</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D48" t="s">
         <v>7</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E48" t="s">
         <v>21</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F48" t="s">
         <v>65</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G48" t="s">
         <v>66</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H48" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
backlog bijgewerkt voor vrijdag ochtend
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Case_BPM2\Case_BPM3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A331F9-C51E-4218-8ACC-0D4802BABB9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38FF67A-A096-4FD1-A6AF-82D0ABC5D898}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1284" windowWidth="17280" windowHeight="8964" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="2664" windowWidth="17280" windowHeight="8964" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cursusadministatie User Stories" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="143">
   <si>
     <t>Cursussen invoeren</t>
   </si>
@@ -601,6 +601,24 @@
   </si>
   <si>
     <t>Unit tests voor oude controller omschrijven naar repository</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Feedback van product owner over foutmeldingen verwerken</t>
+  </si>
+  <si>
+    <t>weeknummer en jaar los invullen</t>
+  </si>
+  <si>
+    <t>Hoofdpagina maken van de huidige week</t>
+  </si>
+  <si>
+    <t>readme.md aanmaken en met instructie vullen</t>
+  </si>
+  <si>
+    <t>testen op andere pc</t>
   </si>
 </sst>
 </file>
@@ -833,7 +851,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -908,6 +926,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -968,7 +987,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1339,11 +1358,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
       <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1387,14 +1406,14 @@
       <c r="AH2"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1487,11 +1506,11 @@
       <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="40"/>
       <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
@@ -1515,9 +1534,9 @@
       <c r="AJ8" s="4"/>
     </row>
     <row r="9" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="46"/>
       <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
@@ -1543,11 +1562,11 @@
       <c r="AJ10" s="22"/>
     </row>
     <row r="11" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
       <c r="I11" s="17" t="s">
         <v>38</v>
       </c>
@@ -1565,9 +1584,9 @@
       <c r="AJ11" s="4"/>
     </row>
     <row r="12" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
       <c r="I12" s="7" t="s">
         <v>39</v>
       </c>
@@ -1585,9 +1604,9 @@
       <c r="AJ12" s="4"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
       <c r="J13" s="4"/>
       <c r="W13"/>
       <c r="X13"/>
@@ -1596,9 +1615,9 @@
       <c r="AJ13" s="4"/>
     </row>
     <row r="14" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="J14" s="4"/>
       <c r="S14" s="17" t="s">
         <v>27</v>
@@ -1613,11 +1632,11 @@
       <c r="AJ14" s="4"/>
     </row>
     <row r="15" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
       <c r="J15" s="4"/>
-      <c r="S15" s="46" t="s">
+      <c r="S15" s="47" t="s">
         <v>83</v>
       </c>
       <c r="U15" s="19" t="s">
@@ -1632,16 +1651,16 @@
     <row r="16" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
-      <c r="S16" s="47"/>
+      <c r="S16" s="48"/>
       <c r="AI16" s="22"/>
       <c r="AJ16" s="22"/>
     </row>
     <row r="17" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
       <c r="I17" s="17" t="s">
         <v>48</v>
       </c>
@@ -1653,9 +1672,9 @@
       <c r="AJ17" s="4"/>
     </row>
     <row r="18" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="42"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
       <c r="I18" s="8" t="s">
         <v>49</v>
       </c>
@@ -1667,9 +1686,9 @@
       <c r="AJ18" s="4"/>
     </row>
     <row r="19" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="42"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="W19"/>
@@ -1679,9 +1698,9 @@
       <c r="AJ19" s="4"/>
     </row>
     <row r="20" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
       <c r="G20" s="17" t="s">
         <v>56</v>
       </c>
@@ -1696,9 +1715,9 @@
       <c r="AJ20" s="4"/>
     </row>
     <row r="21" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
       <c r="G21" s="18"/>
       <c r="I21" s="19" t="s">
         <v>58</v>
@@ -1711,9 +1730,9 @@
       <c r="AJ21" s="4"/>
     </row>
     <row r="22" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="42"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="W22"/>
@@ -1723,9 +1742,9 @@
       <c r="AJ22" s="4"/>
     </row>
     <row r="23" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="42"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
       <c r="G23" s="17" t="s">
         <v>80</v>
       </c>
@@ -1738,9 +1757,9 @@
       <c r="AJ23" s="4"/>
     </row>
     <row r="24" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="43"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
       <c r="G24" s="19" t="s">
         <v>81</v>
       </c>
@@ -1778,11 +1797,11 @@
       <c r="AJ25" s="22"/>
     </row>
     <row r="26" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="40"/>
       <c r="G26" s="17" t="s">
         <v>64</v>
       </c>
@@ -1801,9 +1820,9 @@
       <c r="AJ26" s="4"/>
     </row>
     <row r="27" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
       <c r="G27" s="18"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1826,11 +1845,11 @@
       <c r="AJ28" s="22"/>
     </row>
     <row r="29" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
       <c r="J29" s="4"/>
       <c r="W29" s="17" t="s">
         <v>8</v>
@@ -1847,9 +1866,9 @@
       <c r="AJ29" s="4"/>
     </row>
     <row r="30" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="43"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="46"/>
       <c r="J30" s="4"/>
       <c r="W30" s="8" t="s">
         <v>30</v>
@@ -1865,9 +1884,9 @@
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:36" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="39"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="40"/>
       <c r="I32" s="17" t="s">
         <v>70</v>
       </c>
@@ -1878,9 +1897,9 @@
       <c r="AH32" s="4"/>
     </row>
     <row r="33" spans="1:34" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
       <c r="I33" s="19" t="s">
         <v>71</v>
       </c>
@@ -1891,9 +1910,9 @@
       <c r="AH33" s="4"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="43"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -1912,9 +1931,9 @@
       <c r="AH34" s="4"/>
     </row>
     <row r="35" spans="1:34" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="42"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="43"/>
       <c r="K35" s="17" t="s">
         <v>8</v>
       </c>
@@ -1931,9 +1950,9 @@
       <c r="AH35" s="4"/>
     </row>
     <row r="36" spans="1:34" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="43"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="45"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
       <c r="K36" s="8" t="s">
         <v>30</v>
       </c>
@@ -2233,10 +2252,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2470,29 +2489,29 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+    <row r="14" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="28">
         <v>2</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="28">
         <v>2</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="48" t="s">
+      <c r="H14" s="28" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2601,6 +2620,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" s="26" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>95</v>
+      </c>
       <c r="D19" s="26" t="s">
         <v>0</v>
       </c>
@@ -2612,6 +2634,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" s="26" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
+        <v>95</v>
+      </c>
       <c r="D20" s="26" t="s">
         <v>0</v>
       </c>
@@ -2622,353 +2647,269 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
+    <row r="21" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="28">
         <v>5</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="28">
         <v>2</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="48" t="s">
+      <c r="H21" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="26">
+        <v>5</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B22">
+      <c r="B23" s="26">
         <v>6</v>
       </c>
-      <c r="C22">
+      <c r="C23" s="26">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B23">
+      <c r="B24" s="26">
         <v>7</v>
       </c>
-      <c r="C23">
+      <c r="C24" s="26">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B24">
+      <c r="B25" s="26">
         <v>7</v>
       </c>
-      <c r="C24">
+      <c r="C25" s="26">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+    <row r="26" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="49" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B30" s="28">
         <v>8</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C30" s="28">
         <v>1</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D30" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E30" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="F30" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="G30" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H30" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B26">
+      <c r="B31" s="26">
         <v>9</v>
       </c>
-      <c r="C26">
+      <c r="C31" s="26">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D31" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E31" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F31" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="H26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27">
-        <v>10</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" t="s">
-        <v>102</v>
-      </c>
-      <c r="H27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="23">
-        <v>10</v>
-      </c>
-      <c r="C28" s="23">
-        <v>2</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H28" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29">
-        <v>11</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30">
-        <v>11</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="23">
-        <v>11</v>
-      </c>
-      <c r="C31" s="23">
-        <v>3</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="23" t="s">
+      <c r="H31" s="26" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B32">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="G32" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="H32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33">
-        <v>12</v>
-      </c>
-      <c r="C33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="23">
+        <v>10</v>
+      </c>
+      <c r="C33" s="23">
+        <v>2</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" t="s">
-        <v>41</v>
-      </c>
-      <c r="G33" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" t="s">
-        <v>23</v>
+      <c r="F33" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B34">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H34" t="s">
         <v>23</v>
@@ -2976,129 +2917,123 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36">
-        <v>14</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" t="s">
-        <v>43</v>
-      </c>
-      <c r="H36" t="s">
+    <row r="36" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="23">
+        <v>11</v>
+      </c>
+      <c r="C36" s="23">
+        <v>3</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B37">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
-        <v>9</v>
-      </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="H37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="23">
-        <v>14</v>
-      </c>
-      <c r="C38" s="23">
-        <v>4</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="23" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38">
         <v>12</v>
       </c>
-      <c r="F38" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H38" s="23" t="s">
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G39" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H39" t="s">
         <v>23</v>
@@ -3106,25 +3041,25 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B40">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E40" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="H40" t="s">
         <v>23</v>
@@ -3132,79 +3067,79 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B41">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F42" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="G42" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43">
-        <v>16</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="23">
+        <v>14</v>
+      </c>
+      <c r="C43" s="23">
+        <v>4</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3213,22 +3148,22 @@
         <v>109</v>
       </c>
       <c r="B44">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="G44" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H44" t="s">
         <v>23</v>
@@ -3236,10 +3171,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B45">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C45">
         <v>3</v>
@@ -3248,13 +3183,13 @@
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F45" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G45" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H45" t="s">
         <v>23</v>
@@ -3262,79 +3197,209 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B46">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
         <v>3</v>
       </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" t="s">
-        <v>21</v>
-      </c>
       <c r="F46" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="G46" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="H46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B47">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="H47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48">
+        <v>16</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" t="s">
+        <v>40</v>
+      </c>
+      <c r="H48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" t="s">
+        <v>51</v>
+      </c>
+      <c r="H49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" t="s">
+        <v>59</v>
+      </c>
+      <c r="H50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51">
+        <v>17</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>111</v>
       </c>
-      <c r="B48">
+      <c r="B52">
+        <v>18</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
         <v>19</v>
       </c>
-      <c r="C48">
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" t="s">
+        <v>59</v>
+      </c>
+      <c r="H52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53">
+        <v>19</v>
+      </c>
+      <c r="C53">
         <v>3</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D53" t="s">
         <v>7</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E53" t="s">
         <v>21</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F53" t="s">
         <v>65</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G53" t="s">
         <v>66</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H53" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
in principe naar weeknummer pagina gaan
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Case_BPM2\Case_BPM3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38FF67A-A096-4FD1-A6AF-82D0ABC5D898}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF48409D-2390-4F3C-BC21-B3B7ED47BB35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="2664" windowWidth="17280" windowHeight="8964" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="1536" windowWidth="17280" windowHeight="8964" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cursusadministatie User Stories" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="146">
   <si>
     <t>Cursussen invoeren</t>
   </si>
@@ -487,9 +487,6 @@
     <t>3 - geimporteerde lijst gesorteerd per week weergeven</t>
   </si>
   <si>
-    <t>lijst in gekozen week tonen</t>
-  </si>
-  <si>
     <t>4 - Alleen cursusinstanties binnen periode importeren EN navigeren naar volgende en vorige week</t>
   </si>
   <si>
@@ -618,7 +615,19 @@
     <t>readme.md aanmaken en met instructie vullen</t>
   </si>
   <si>
-    <t>testen op andere pc</t>
+    <t>Exploratory testen</t>
+  </si>
+  <si>
+    <t>Extra testen toevoegen</t>
+  </si>
+  <si>
+    <t>Pagina layout (Bootstrap-CSS)</t>
+  </si>
+  <si>
+    <t>Weeknummer maximum dynamisch aanpassen i.p.v. melding</t>
+  </si>
+  <si>
+    <t>testen op een andere pc vanaf github</t>
   </si>
 </sst>
 </file>
@@ -679,7 +688,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,6 +746,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,7 +872,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -987,7 +1008,8 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1984,7 +2006,7 @@
     </row>
     <row r="39" spans="1:34" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AC39" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AD39" s="4"/>
       <c r="AE39" s="19" t="s">
@@ -1992,7 +2014,7 @@
       </c>
       <c r="AF39" s="4"/>
       <c r="AG39" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:34" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -2059,7 +2081,7 @@
       <c r="Z42" s="4"/>
       <c r="AB42" s="4"/>
       <c r="AC42" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AD42" s="4"/>
       <c r="AE42" s="24" t="s">
@@ -2153,7 +2175,7 @@
       </c>
       <c r="AF45" s="4"/>
       <c r="AG45" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AH45" s="4"/>
     </row>
@@ -2252,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,35 +2327,35 @@
         <v>1</v>
       </c>
       <c r="D2" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D3" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>124</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D4" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>126</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -2367,13 +2389,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="27" t="s">
         <v>116</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -2381,13 +2403,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>116</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -2441,10 +2463,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>131</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -2452,13 +2474,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -2466,13 +2488,13 @@
         <v>2</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -2480,13 +2502,13 @@
         <v>2</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -2627,10 +2649,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>133</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="26" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2641,10 +2663,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>135</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -2681,10 +2703,10 @@
         <v>5</v>
       </c>
       <c r="E22" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="26" t="s">
         <v>137</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -2736,252 +2758,177 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="26">
-        <v>7</v>
-      </c>
-      <c r="C25" s="26">
+      <c r="B25" s="28">
+        <v>8</v>
+      </c>
+      <c r="C25" s="28">
         <v>1</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="26">
+        <v>9</v>
+      </c>
+      <c r="C26" s="26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="49" t="s">
+      <c r="F27" s="26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="49" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="49" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="49" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="49" t="s">
+    <row r="34" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="50" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="28">
-        <v>8</v>
-      </c>
-      <c r="C30" s="28">
-        <v>1</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" s="26">
-        <v>9</v>
-      </c>
-      <c r="C31" s="26">
-        <v>1</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32">
-        <v>10</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" t="s">
-        <v>102</v>
-      </c>
-      <c r="H32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="23">
-        <v>10</v>
-      </c>
-      <c r="C33" s="23">
-        <v>2</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34">
-        <v>11</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>31</v>
+        <v>100</v>
+      </c>
+      <c r="G35" t="s">
+        <v>101</v>
       </c>
       <c r="H35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B36" s="23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C36" s="23">
+        <v>2</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>20</v>
-      </c>
       <c r="F36" s="23" t="s">
-        <v>32</v>
+        <v>102</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="H36" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B37">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="H37" t="s">
         <v>23</v>
@@ -2989,10 +2936,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -3001,65 +2948,59 @@
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
-      </c>
-      <c r="G38" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>107</v>
-      </c>
-      <c r="B39">
-        <v>13</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" t="s">
-        <v>33</v>
-      </c>
-      <c r="H39" t="s">
+    <row r="39" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="23">
+        <v>11</v>
+      </c>
+      <c r="C39" s="23">
+        <v>3</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H39" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B40">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="G40" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="H40" t="s">
         <v>23</v>
@@ -3067,25 +3008,25 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B41">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="G41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H41" t="s">
         <v>23</v>
@@ -3093,77 +3034,77 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B42">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G42" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B43" s="23">
-        <v>14</v>
-      </c>
-      <c r="C43" s="23">
-        <v>4</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G43" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H43" s="23" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B44">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H44" t="s">
         <v>23</v>
@@ -3171,103 +3112,103 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B45">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F45" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G45" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46">
-        <v>16</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" t="s">
-        <v>105</v>
-      </c>
-      <c r="G46" t="s">
-        <v>68</v>
-      </c>
-      <c r="H46" t="s">
-        <v>22</v>
+    <row r="46" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" s="23">
+        <v>14</v>
+      </c>
+      <c r="C46" s="23">
+        <v>4</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F47" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G47" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="H47" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B48">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F48" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G48" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H48" t="s">
         <v>23</v>
@@ -3275,77 +3216,77 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B49">
         <v>16</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="G49" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="H49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50">
-        <v>17</v>
-      </c>
-      <c r="C50">
-        <v>3</v>
-      </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" t="s">
-        <v>59</v>
-      </c>
-      <c r="H50" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="26">
+        <v>16</v>
+      </c>
+      <c r="C50" s="26">
+        <v>2</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B51">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E51" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="G51" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H51" t="s">
         <v>23</v>
@@ -3353,25 +3294,25 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="G52" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H52" t="s">
         <v>23</v>
@@ -3379,10 +3320,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B53">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -3391,15 +3332,93 @@
         <v>7</v>
       </c>
       <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54">
+        <v>17</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
         <v>21</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
+        <v>53</v>
+      </c>
+      <c r="G54" t="s">
+        <v>52</v>
+      </c>
+      <c r="H54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55">
+        <v>18</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" t="s">
+        <v>59</v>
+      </c>
+      <c r="H55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56">
+        <v>19</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" t="s">
         <v>65</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G56" t="s">
         <v>66</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H56" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>